<commit_message>
New layout. Updated queries. New evaluation
</commit_message>
<xml_diff>
--- a/Example/Filled/2023_Q3___BSP_AR1_ST.w.8.7.5.xlsx
+++ b/Example/Filled/2023_Q3___BSP_AR1_ST.w.8.7.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krzysztof kaniewski\PycharmProjects\pythonProject\Example\Filled\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053243FD-12B4-46F9-B596-DDECC16E1C08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7945CF9-7193-4B28-86A3-F3562116B5A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="830" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="830" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wstęp" sheetId="1" r:id="rId1"/>
@@ -12460,7 +12460,7 @@
   </sheetPr>
   <dimension ref="A1:WVX968"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -26167,8 +26167,8 @@
   </sheetPr>
   <dimension ref="A1:WSW40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AC26" sqref="AC25:AC26"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28060,6 +28060,7 @@
       <c r="D40" s="1"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="D1fRq0KcssiAutIEWvKgaH3PJGKGtyvdw5XSbvIltU2XU4gBiadQgWMAevzvMIH5XIVsZSXvtxUcaK5Ehc5/Ow==" saltValue="J+W2OJ0SJnqgfopcmtTtCQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="34">
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="T5:U5"/>
@@ -28108,8 +28109,8 @@
   </sheetPr>
   <dimension ref="A1:T570"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28277,7 +28278,7 @@
         <v>53</v>
       </c>
       <c r="N10" s="185">
-        <v>11771</v>
+        <v>12044</v>
       </c>
       <c r="O10" s="185">
         <v>0</v>
@@ -28286,7 +28287,7 @@
         <v>15</v>
       </c>
       <c r="Q10" s="186">
-        <v>1008904.24</v>
+        <v>1247194.71</v>
       </c>
       <c r="R10" s="186">
         <v>0</v>
@@ -28313,7 +28314,7 @@
         <v>70</v>
       </c>
       <c r="N11" s="185">
-        <v>31662</v>
+        <v>31923</v>
       </c>
       <c r="O11" s="185">
         <v>0</v>
@@ -28322,7 +28323,7 @@
         <v>2</v>
       </c>
       <c r="Q11" s="186">
-        <v>2701615.24</v>
+        <v>2929628.08</v>
       </c>
       <c r="R11" s="186">
         <v>0</v>
@@ -28349,7 +28350,7 @@
         <v>75</v>
       </c>
       <c r="N12" s="185">
-        <v>2021</v>
+        <v>2043</v>
       </c>
       <c r="O12" s="185">
         <v>0</v>
@@ -28358,7 +28359,7 @@
         <v>1</v>
       </c>
       <c r="Q12" s="186">
-        <v>131092.17000000001</v>
+        <v>160105.29999999999</v>
       </c>
       <c r="R12" s="186">
         <v>0</v>
@@ -28385,7 +28386,7 @@
         <v>286</v>
       </c>
       <c r="N13" s="185">
-        <v>995</v>
+        <v>999</v>
       </c>
       <c r="O13" s="185">
         <v>0</v>
@@ -28394,7 +28395,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="186">
-        <v>63899.18</v>
+        <v>81548.179999999993</v>
       </c>
       <c r="R13" s="186">
         <v>0</v>
@@ -28421,7 +28422,7 @@
         <v>164</v>
       </c>
       <c r="N14" s="185">
-        <v>783</v>
+        <v>799</v>
       </c>
       <c r="O14" s="185">
         <v>0</v>
@@ -28430,7 +28431,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="186">
-        <v>73813.36</v>
+        <v>95664.44</v>
       </c>
       <c r="R14" s="186">
         <v>0</v>
@@ -28457,7 +28458,7 @@
         <v>167</v>
       </c>
       <c r="N15" s="185">
-        <v>114240</v>
+        <v>115747</v>
       </c>
       <c r="O15" s="185">
         <v>0</v>
@@ -28466,7 +28467,7 @@
         <v>8</v>
       </c>
       <c r="Q15" s="186">
-        <v>9660057.6500000004</v>
+        <v>11451012.369999999</v>
       </c>
       <c r="R15" s="186">
         <v>0</v>
@@ -28493,7 +28494,7 @@
         <v>177</v>
       </c>
       <c r="N16" s="185">
-        <v>25070</v>
+        <v>25428</v>
       </c>
       <c r="O16" s="185">
         <v>0</v>
@@ -28502,7 +28503,7 @@
         <v>22</v>
       </c>
       <c r="Q16" s="186">
-        <v>2287011.85</v>
+        <v>2712145.5</v>
       </c>
       <c r="R16" s="186">
         <v>0</v>
@@ -28529,7 +28530,7 @@
         <v>194</v>
       </c>
       <c r="N17" s="185">
-        <v>5066</v>
+        <v>5154</v>
       </c>
       <c r="O17" s="185">
         <v>0</v>
@@ -28538,7 +28539,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="186">
-        <v>358700.21</v>
+        <v>436433.52</v>
       </c>
       <c r="R17" s="186">
         <v>0</v>
@@ -28565,7 +28566,7 @@
         <v>212</v>
       </c>
       <c r="N18" s="185">
-        <v>7652</v>
+        <v>7687</v>
       </c>
       <c r="O18" s="185">
         <v>0</v>
@@ -28574,7 +28575,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="186">
-        <v>487556.29</v>
+        <v>517467.66</v>
       </c>
       <c r="R18" s="186">
         <v>0</v>
@@ -28601,7 +28602,7 @@
         <v>228</v>
       </c>
       <c r="N19" s="185">
-        <v>19003</v>
+        <v>19179</v>
       </c>
       <c r="O19" s="185">
         <v>0</v>
@@ -28610,7 +28611,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="186">
-        <v>1910668.76</v>
+        <v>2079236.3</v>
       </c>
       <c r="R19" s="186">
         <v>0</v>
@@ -28637,7 +28638,7 @@
         <v>261</v>
       </c>
       <c r="N20" s="185">
-        <v>1620</v>
+        <v>1637</v>
       </c>
       <c r="O20" s="185">
         <v>0</v>
@@ -28646,7 +28647,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="186">
-        <v>88350.43</v>
+        <v>107086.43</v>
       </c>
       <c r="R20" s="186">
         <v>0</v>
@@ -28673,7 +28674,7 @@
         <v>205</v>
       </c>
       <c r="N21" s="185">
-        <v>14272</v>
+        <v>14386</v>
       </c>
       <c r="O21" s="185">
         <v>0</v>
@@ -28682,7 +28683,7 @@
         <v>0</v>
       </c>
       <c r="Q21" s="186">
-        <v>989713.31</v>
+        <v>1098119.8500000001</v>
       </c>
       <c r="R21" s="186">
         <v>0</v>
@@ -28709,7 +28710,7 @@
         <v>470</v>
       </c>
       <c r="N22" s="185">
-        <v>62749</v>
+        <v>63794</v>
       </c>
       <c r="O22" s="185">
         <v>0</v>
@@ -28718,7 +28719,7 @@
         <v>17</v>
       </c>
       <c r="Q22" s="186">
-        <v>4691380.83</v>
+        <v>5657696.5199999996</v>
       </c>
       <c r="R22" s="186">
         <v>0</v>
@@ -28745,7 +28746,7 @@
         <v>297</v>
       </c>
       <c r="N23" s="185">
-        <v>31329</v>
+        <v>31850</v>
       </c>
       <c r="O23" s="185">
         <v>0</v>
@@ -28754,7 +28755,7 @@
         <v>1</v>
       </c>
       <c r="Q23" s="186">
-        <v>7133898.9299999997</v>
+        <v>7707619.8300000001</v>
       </c>
       <c r="R23" s="186">
         <v>0</v>
@@ -28781,7 +28782,7 @@
         <v>320</v>
       </c>
       <c r="N24" s="185">
-        <v>9274</v>
+        <v>9381</v>
       </c>
       <c r="O24" s="185">
         <v>0</v>
@@ -28790,7 +28791,7 @@
         <v>1</v>
       </c>
       <c r="Q24" s="186">
-        <v>842574.46</v>
+        <v>961836.05</v>
       </c>
       <c r="R24" s="186">
         <v>0</v>
@@ -28853,7 +28854,7 @@
         <v>387</v>
       </c>
       <c r="N26" s="185">
-        <v>33878</v>
+        <v>34664</v>
       </c>
       <c r="O26" s="185">
         <v>0</v>
@@ -28862,7 +28863,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="186">
-        <v>2581082.7999999998</v>
+        <v>3251422.15</v>
       </c>
       <c r="R26" s="186">
         <v>0</v>
@@ -28889,7 +28890,7 @@
         <v>390</v>
       </c>
       <c r="N27" s="185">
-        <v>1569</v>
+        <v>1579</v>
       </c>
       <c r="O27" s="185">
         <v>0</v>
@@ -28898,7 +28899,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="186">
-        <v>209624.08</v>
+        <v>220949.43</v>
       </c>
       <c r="R27" s="186">
         <v>0</v>
@@ -28925,7 +28926,7 @@
         <v>393</v>
       </c>
       <c r="N28" s="185">
-        <v>6759</v>
+        <v>6842</v>
       </c>
       <c r="O28" s="185">
         <v>0</v>
@@ -28934,7 +28935,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="186">
-        <v>484218.17</v>
+        <v>576723.80000000005</v>
       </c>
       <c r="R28" s="186">
         <v>0</v>
@@ -28961,7 +28962,7 @@
         <v>436</v>
       </c>
       <c r="N29" s="185">
-        <v>692</v>
+        <v>708</v>
       </c>
       <c r="O29" s="185">
         <v>0</v>
@@ -28970,7 +28971,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="186">
-        <v>46538.85</v>
+        <v>67526.880000000005</v>
       </c>
       <c r="R29" s="186">
         <v>0</v>
@@ -28997,7 +28998,7 @@
         <v>170</v>
       </c>
       <c r="N30" s="185">
-        <v>169824</v>
+        <v>176494</v>
       </c>
       <c r="O30" s="185">
         <v>0</v>
@@ -29006,7 +29007,7 @@
         <v>55</v>
       </c>
       <c r="Q30" s="186">
-        <v>20379033.370000001</v>
+        <v>26708456.82</v>
       </c>
       <c r="R30" s="186">
         <v>0</v>
@@ -29033,7 +29034,7 @@
         <v>474</v>
       </c>
       <c r="N31" s="185">
-        <v>58399</v>
+        <v>58775</v>
       </c>
       <c r="O31" s="185">
         <v>0</v>
@@ -29042,7 +29043,7 @@
         <v>2</v>
       </c>
       <c r="Q31" s="186">
-        <v>5954306.2999999998</v>
+        <v>6390818.46</v>
       </c>
       <c r="R31" s="186">
         <v>0</v>
@@ -29069,7 +29070,7 @@
         <v>514</v>
       </c>
       <c r="N32" s="185">
-        <v>1775</v>
+        <v>1793</v>
       </c>
       <c r="O32" s="185">
         <v>0</v>
@@ -29078,7 +29079,7 @@
         <v>0</v>
       </c>
       <c r="Q32" s="186">
-        <v>132829.01</v>
+        <v>162375.63</v>
       </c>
       <c r="R32" s="186">
         <v>0</v>
@@ -29105,7 +29106,7 @@
         <v>526</v>
       </c>
       <c r="N33" s="185">
-        <v>4536</v>
+        <v>4581</v>
       </c>
       <c r="O33" s="185">
         <v>0</v>
@@ -29114,7 +29115,7 @@
         <v>1</v>
       </c>
       <c r="Q33" s="186">
-        <v>292066.55</v>
+        <v>354481.38</v>
       </c>
       <c r="R33" s="186">
         <v>0</v>
@@ -29141,7 +29142,7 @@
         <v>563</v>
       </c>
       <c r="N34" s="185">
-        <v>27796</v>
+        <v>27988</v>
       </c>
       <c r="O34" s="185">
         <v>0</v>
@@ -29150,7 +29151,7 @@
         <v>0</v>
       </c>
       <c r="Q34" s="186">
-        <v>2370012.08</v>
+        <v>2562380.91</v>
       </c>
       <c r="R34" s="186">
         <v>0</v>
@@ -29177,7 +29178,7 @@
         <v>557</v>
       </c>
       <c r="N35" s="185">
-        <v>1054</v>
+        <v>1068</v>
       </c>
       <c r="O35" s="185">
         <v>0</v>
@@ -29186,7 +29187,7 @@
         <v>0</v>
       </c>
       <c r="Q35" s="186">
-        <v>62873.74</v>
+        <v>76924.12</v>
       </c>
       <c r="R35" s="186">
         <v>0</v>
@@ -29213,7 +29214,7 @@
         <v>548</v>
       </c>
       <c r="N36" s="185">
-        <v>42104</v>
+        <v>42865</v>
       </c>
       <c r="O36" s="185">
         <v>0</v>
@@ -29222,7 +29223,7 @@
         <v>1</v>
       </c>
       <c r="Q36" s="186">
-        <v>3254563.86</v>
+        <v>4112712.57</v>
       </c>
       <c r="R36" s="186">
         <v>0</v>
@@ -29249,7 +29250,7 @@
         <v>291</v>
       </c>
       <c r="N37" s="185">
-        <v>4217</v>
+        <v>4294</v>
       </c>
       <c r="O37" s="185">
         <v>0</v>
@@ -29258,7 +29259,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="186">
-        <v>241890.73</v>
+        <v>328579.32</v>
       </c>
       <c r="R37" s="186">
         <v>0</v>
@@ -29285,7 +29286,7 @@
         <v>323</v>
       </c>
       <c r="N38" s="185">
-        <v>17685</v>
+        <v>17960</v>
       </c>
       <c r="O38" s="185">
         <v>0</v>
@@ -29294,7 +29295,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="186">
-        <v>1245771.56</v>
+        <v>1475138.77</v>
       </c>
       <c r="R38" s="186">
         <v>0</v>
@@ -29326,7 +29327,7 @@
       </c>
       <c r="N39" s="185">
         <f t="shared" ref="N39:S39" si="0">SUM(N40:N1048576)</f>
-        <v>1048503</v>
+        <v>1054168</v>
       </c>
       <c r="O39" s="185">
         <f t="shared" si="0"/>
@@ -29338,7 +29339,7 @@
       </c>
       <c r="Q39" s="186">
         <f t="shared" si="0"/>
-        <v>68624285.840000004</v>
+        <v>79252315.540000007</v>
       </c>
       <c r="R39" s="186">
         <f t="shared" si="0"/>
@@ -29367,7 +29368,8 @@
         <v>947</v>
       </c>
       <c r="N40" s="185">
-        <v>593942</v>
+        <f>595745+1</f>
+        <v>595746</v>
       </c>
       <c r="O40" s="185">
         <v>0</v>
@@ -29376,7 +29378,8 @@
         <v>11</v>
       </c>
       <c r="Q40" s="186">
-        <v>36464493.210000001</v>
+        <f>38322657.12+170</f>
+        <v>38322827.119999997</v>
       </c>
       <c r="R40" s="186">
         <v>0</v>
@@ -29396,7 +29399,7 @@
         <v>694</v>
       </c>
       <c r="N41" s="187">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="O41" s="187">
         <v>0</v>
@@ -29405,7 +29408,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="188">
-        <v>20872.02</v>
+        <v>21472.02</v>
       </c>
       <c r="R41" s="188">
         <v>0</v>
@@ -29425,7 +29428,7 @@
         <v>37</v>
       </c>
       <c r="N42" s="187">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O42" s="187">
         <v>0</v>
@@ -29434,7 +29437,7 @@
         <v>0</v>
       </c>
       <c r="Q42" s="188">
-        <v>2560.84</v>
+        <v>3015.84</v>
       </c>
       <c r="R42" s="188">
         <v>0</v>
@@ -29546,7 +29549,7 @@
         <v>47</v>
       </c>
       <c r="N46" s="187">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="O46" s="187">
         <v>0</v>
@@ -29555,7 +29558,7 @@
         <v>0</v>
       </c>
       <c r="Q46" s="188">
-        <v>13562.35</v>
+        <v>14032.35</v>
       </c>
       <c r="R46" s="188">
         <v>0</v>
@@ -29575,7 +29578,7 @@
         <v>39</v>
       </c>
       <c r="N47" s="187">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="O47" s="187">
         <v>0</v>
@@ -29584,7 +29587,7 @@
         <v>0</v>
       </c>
       <c r="Q47" s="188">
-        <v>13972.05</v>
+        <v>19840.93</v>
       </c>
       <c r="R47" s="188">
         <v>0</v>
@@ -29633,7 +29636,7 @@
         <v>55</v>
       </c>
       <c r="N49" s="187">
-        <v>6956</v>
+        <v>7054</v>
       </c>
       <c r="O49" s="187">
         <v>0</v>
@@ -29642,7 +29645,7 @@
         <v>0</v>
       </c>
       <c r="Q49" s="188">
-        <v>510121.9</v>
+        <v>739911.33</v>
       </c>
       <c r="R49" s="188">
         <v>0</v>
@@ -29662,7 +29665,7 @@
         <v>59</v>
       </c>
       <c r="N50" s="187">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="O50" s="187">
         <v>0</v>
@@ -29671,7 +29674,7 @@
         <v>0</v>
       </c>
       <c r="Q50" s="188">
-        <v>71261.279999999999</v>
+        <v>75051.240000000005</v>
       </c>
       <c r="R50" s="188">
         <v>0</v>
@@ -29720,7 +29723,7 @@
         <v>78</v>
       </c>
       <c r="N52" s="187">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="O52" s="187">
         <v>0</v>
@@ -29729,7 +29732,7 @@
         <v>0</v>
       </c>
       <c r="Q52" s="188">
-        <v>13941.48</v>
+        <v>15731.84</v>
       </c>
       <c r="R52" s="188">
         <v>0</v>
@@ -29807,7 +29810,7 @@
         <v>109</v>
       </c>
       <c r="N55" s="187">
-        <v>18073</v>
+        <v>18352</v>
       </c>
       <c r="O55" s="187">
         <v>0</v>
@@ -29816,7 +29819,7 @@
         <v>2</v>
       </c>
       <c r="Q55" s="188">
-        <v>918101.72</v>
+        <v>4481773.6900000004</v>
       </c>
       <c r="R55" s="188">
         <v>0</v>
@@ -29865,7 +29868,7 @@
         <v>85</v>
       </c>
       <c r="N57" s="187">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O57" s="187">
         <v>0</v>
@@ -29874,7 +29877,7 @@
         <v>0</v>
       </c>
       <c r="Q57" s="188">
-        <v>1383.33</v>
+        <v>25803.33</v>
       </c>
       <c r="R57" s="188">
         <v>0</v>
@@ -29923,7 +29926,7 @@
         <v>62</v>
       </c>
       <c r="N59" s="187">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="O59" s="187">
         <v>0</v>
@@ -29932,7 +29935,7 @@
         <v>0</v>
       </c>
       <c r="Q59" s="188">
-        <v>8652.99</v>
+        <v>10102.99</v>
       </c>
       <c r="R59" s="188">
         <v>0</v>
@@ -29981,7 +29984,7 @@
         <v>96</v>
       </c>
       <c r="N61" s="187">
-        <v>1274</v>
+        <v>1278</v>
       </c>
       <c r="O61" s="187">
         <v>0</v>
@@ -29990,7 +29993,7 @@
         <v>0</v>
       </c>
       <c r="Q61" s="188">
-        <v>74995.19</v>
+        <v>78197.990000000005</v>
       </c>
       <c r="R61" s="188">
         <v>0</v>
@@ -30126,7 +30129,7 @@
         <v>114</v>
       </c>
       <c r="N66" s="187">
-        <v>7685</v>
+        <v>7764</v>
       </c>
       <c r="O66" s="187">
         <v>0</v>
@@ -30135,7 +30138,7 @@
         <v>0</v>
       </c>
       <c r="Q66" s="188">
-        <v>807501.86</v>
+        <v>895573.63</v>
       </c>
       <c r="R66" s="188">
         <v>0</v>
@@ -30213,7 +30216,7 @@
         <v>143</v>
       </c>
       <c r="N69" s="187">
-        <v>1993</v>
+        <v>2002</v>
       </c>
       <c r="O69" s="187">
         <v>0</v>
@@ -30222,7 +30225,7 @@
         <v>0</v>
       </c>
       <c r="Q69" s="188">
-        <v>178540.39</v>
+        <v>187159.39</v>
       </c>
       <c r="R69" s="188">
         <v>0</v>
@@ -30242,7 +30245,7 @@
         <v>146</v>
       </c>
       <c r="N70" s="187">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="O70" s="187">
         <v>0</v>
@@ -30251,7 +30254,7 @@
         <v>0</v>
       </c>
       <c r="Q70" s="188">
-        <v>32179.360000000001</v>
+        <v>34207.160000000003</v>
       </c>
       <c r="R70" s="188">
         <v>0</v>
@@ -30329,7 +30332,7 @@
         <v>149</v>
       </c>
       <c r="N73" s="187">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="O73" s="187">
         <v>0</v>
@@ -30338,7 +30341,7 @@
         <v>0</v>
       </c>
       <c r="Q73" s="188">
-        <v>21201.11</v>
+        <v>24280.2</v>
       </c>
       <c r="R73" s="188">
         <v>0</v>
@@ -30503,7 +30506,7 @@
         <v>196</v>
       </c>
       <c r="N79" s="187">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="O79" s="187">
         <v>0</v>
@@ -30512,7 +30515,7 @@
         <v>0</v>
       </c>
       <c r="Q79" s="188">
-        <v>64431.11</v>
+        <v>72000.44</v>
       </c>
       <c r="R79" s="188">
         <v>0</v>
@@ -30619,7 +30622,7 @@
         <v>240</v>
       </c>
       <c r="N83" s="187">
-        <v>2998</v>
+        <v>3028</v>
       </c>
       <c r="O83" s="187">
         <v>0</v>
@@ -30628,7 +30631,7 @@
         <v>0</v>
       </c>
       <c r="Q83" s="188">
-        <v>183979.42</v>
+        <v>212607.64</v>
       </c>
       <c r="R83" s="188">
         <v>0</v>
@@ -30764,7 +30767,7 @@
         <v>267</v>
       </c>
       <c r="N88" s="187">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="O88" s="187">
         <v>0</v>
@@ -30773,7 +30776,7 @@
         <v>0</v>
       </c>
       <c r="Q88" s="188">
-        <v>6126.88</v>
+        <v>7099.78</v>
       </c>
       <c r="R88" s="188">
         <v>0</v>
@@ -30851,7 +30854,7 @@
         <v>278</v>
       </c>
       <c r="N91" s="187">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="O91" s="187">
         <v>0</v>
@@ -30860,7 +30863,7 @@
         <v>0</v>
       </c>
       <c r="Q91" s="188">
-        <v>57365.26</v>
+        <v>67124.84</v>
       </c>
       <c r="R91" s="188">
         <v>0</v>
@@ -30880,7 +30883,7 @@
         <v>306</v>
       </c>
       <c r="N92" s="187">
-        <v>1008</v>
+        <v>1016</v>
       </c>
       <c r="O92" s="187">
         <v>0</v>
@@ -30889,7 +30892,7 @@
         <v>0</v>
       </c>
       <c r="Q92" s="188">
-        <v>77024.75</v>
+        <v>95961.35</v>
       </c>
       <c r="R92" s="188">
         <v>0</v>
@@ -30909,7 +30912,7 @@
         <v>294</v>
       </c>
       <c r="N93" s="187">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="O93" s="187">
         <v>0</v>
@@ -30918,7 +30921,7 @@
         <v>0</v>
       </c>
       <c r="Q93" s="188">
-        <v>11901.57</v>
+        <v>12365.57</v>
       </c>
       <c r="R93" s="188">
         <v>0</v>
@@ -30967,7 +30970,7 @@
         <v>300</v>
       </c>
       <c r="N95" s="187">
-        <v>4298</v>
+        <v>4376</v>
       </c>
       <c r="O95" s="187">
         <v>0</v>
@@ -30976,7 +30979,7 @@
         <v>0</v>
       </c>
       <c r="Q95" s="188">
-        <v>385239.44</v>
+        <v>455524.72</v>
       </c>
       <c r="R95" s="188">
         <v>0</v>
@@ -31025,7 +31028,7 @@
         <v>336</v>
       </c>
       <c r="N97" s="187">
-        <v>1236</v>
+        <v>1247</v>
       </c>
       <c r="O97" s="187">
         <v>0</v>
@@ -31034,7 +31037,7 @@
         <v>0</v>
       </c>
       <c r="Q97" s="188">
-        <v>85781.84</v>
+        <v>99726.69</v>
       </c>
       <c r="R97" s="188">
         <v>0</v>
@@ -31083,7 +31086,7 @@
         <v>333</v>
       </c>
       <c r="N99" s="187">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="O99" s="187">
         <v>0</v>
@@ -31092,7 +31095,7 @@
         <v>0</v>
       </c>
       <c r="Q99" s="188">
-        <v>13507.98</v>
+        <v>14007.98</v>
       </c>
       <c r="R99" s="188">
         <v>0</v>
@@ -31112,7 +31115,7 @@
         <v>368</v>
       </c>
       <c r="N100" s="187">
-        <v>2118</v>
+        <v>2124</v>
       </c>
       <c r="O100" s="187">
         <v>0</v>
@@ -31121,7 +31124,7 @@
         <v>0</v>
       </c>
       <c r="Q100" s="188">
-        <v>110823.37</v>
+        <v>114251.1</v>
       </c>
       <c r="R100" s="188">
         <v>0</v>
@@ -31170,7 +31173,7 @@
         <v>359</v>
       </c>
       <c r="N102" s="187">
-        <v>3411</v>
+        <v>3526</v>
       </c>
       <c r="O102" s="187">
         <v>0</v>
@@ -31179,7 +31182,7 @@
         <v>0</v>
       </c>
       <c r="Q102" s="188">
-        <v>562824.71</v>
+        <v>706347.04</v>
       </c>
       <c r="R102" s="188">
         <v>0</v>
@@ -31199,7 +31202,7 @@
         <v>362</v>
       </c>
       <c r="N103" s="187">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="O103" s="187">
         <v>0</v>
@@ -31208,7 +31211,7 @@
         <v>0</v>
       </c>
       <c r="Q103" s="188">
-        <v>55232.82</v>
+        <v>66388.820000000007</v>
       </c>
       <c r="R103" s="188">
         <v>0</v>
@@ -31286,7 +31289,7 @@
         <v>374</v>
       </c>
       <c r="N106" s="187">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="O106" s="187">
         <v>0</v>
@@ -31295,7 +31298,7 @@
         <v>0</v>
       </c>
       <c r="Q106" s="188">
-        <v>978.21</v>
+        <v>5688.21</v>
       </c>
       <c r="R106" s="188">
         <v>0</v>
@@ -31402,7 +31405,7 @@
         <v>448</v>
       </c>
       <c r="N110" s="187">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="O110" s="187">
         <v>0</v>
@@ -31411,7 +31414,7 @@
         <v>0</v>
       </c>
       <c r="Q110" s="188">
-        <v>14269.25</v>
+        <v>16924.25</v>
       </c>
       <c r="R110" s="188">
         <v>0</v>
@@ -31489,7 +31492,7 @@
         <v>438</v>
       </c>
       <c r="N113" s="187">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O113" s="187">
         <v>0</v>
@@ -31498,7 +31501,7 @@
         <v>0</v>
       </c>
       <c r="Q113" s="188">
-        <v>1597.02</v>
+        <v>7465.34</v>
       </c>
       <c r="R113" s="188">
         <v>0</v>
@@ -31518,7 +31521,7 @@
         <v>445</v>
       </c>
       <c r="N114" s="187">
-        <v>1539</v>
+        <v>1550</v>
       </c>
       <c r="O114" s="187">
         <v>0</v>
@@ -31527,7 +31530,7 @@
         <v>0</v>
       </c>
       <c r="Q114" s="188">
-        <v>100583.83</v>
+        <v>108915.15</v>
       </c>
       <c r="R114" s="188">
         <v>0</v>
@@ -31547,7 +31550,7 @@
         <v>403</v>
       </c>
       <c r="N115" s="187">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="O115" s="187">
         <v>0</v>
@@ -31556,7 +31559,7 @@
         <v>0</v>
       </c>
       <c r="Q115" s="188">
-        <v>54883.7</v>
+        <v>69282.350000000006</v>
       </c>
       <c r="R115" s="188">
         <v>0</v>
@@ -31605,7 +31608,7 @@
         <v>406</v>
       </c>
       <c r="N117" s="187">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="O117" s="187">
         <v>0</v>
@@ -31614,7 +31617,7 @@
         <v>0</v>
       </c>
       <c r="Q117" s="188">
-        <v>17949.990000000002</v>
+        <v>20049.990000000002</v>
       </c>
       <c r="R117" s="188">
         <v>0</v>
@@ -31634,7 +31637,7 @@
         <v>399</v>
       </c>
       <c r="N118" s="187">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O118" s="187">
         <v>0</v>
@@ -31643,7 +31646,7 @@
         <v>0</v>
       </c>
       <c r="Q118" s="188">
-        <v>4435.21</v>
+        <v>5035.21</v>
       </c>
       <c r="R118" s="188">
         <v>0</v>
@@ -31779,7 +31782,7 @@
         <v>484</v>
       </c>
       <c r="N123" s="187">
-        <v>980</v>
+        <v>984</v>
       </c>
       <c r="O123" s="187">
         <v>0</v>
@@ -31788,7 +31791,7 @@
         <v>0</v>
       </c>
       <c r="Q123" s="188">
-        <v>66242.42</v>
+        <v>69200.42</v>
       </c>
       <c r="R123" s="188">
         <v>0</v>
@@ -31866,7 +31869,7 @@
         <v>415</v>
       </c>
       <c r="N126" s="187">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="O126" s="187">
         <v>0</v>
@@ -31875,7 +31878,7 @@
         <v>0</v>
       </c>
       <c r="Q126" s="188">
-        <v>16785.91</v>
+        <v>17505.91</v>
       </c>
       <c r="R126" s="188">
         <v>0</v>
@@ -31895,7 +31898,7 @@
         <v>487</v>
       </c>
       <c r="N127" s="187">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="O127" s="187">
         <v>0</v>
@@ -31904,7 +31907,7 @@
         <v>0</v>
       </c>
       <c r="Q127" s="188">
-        <v>22385.55</v>
+        <v>24577.87</v>
       </c>
       <c r="R127" s="188">
         <v>0</v>
@@ -32098,7 +32101,7 @@
         <v>501</v>
       </c>
       <c r="N134" s="187">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="O134" s="187">
         <v>0</v>
@@ -32107,7 +32110,7 @@
         <v>0</v>
       </c>
       <c r="Q134" s="188">
-        <v>16883.080000000002</v>
+        <v>25124.58</v>
       </c>
       <c r="R134" s="188">
         <v>0</v>
@@ -32127,7 +32130,7 @@
         <v>523</v>
       </c>
       <c r="N135" s="187">
-        <v>727</v>
+        <v>735</v>
       </c>
       <c r="O135" s="187">
         <v>0</v>
@@ -32136,7 +32139,7 @@
         <v>0</v>
       </c>
       <c r="Q135" s="188">
-        <v>98035.59</v>
+        <v>105685.75999999999</v>
       </c>
       <c r="R135" s="188">
         <v>0</v>
@@ -32243,7 +32246,7 @@
         <v>536</v>
       </c>
       <c r="N139" s="187">
-        <v>3611</v>
+        <v>3619</v>
       </c>
       <c r="O139" s="187">
         <v>0</v>
@@ -32252,7 +32255,7 @@
         <v>0</v>
       </c>
       <c r="Q139" s="188">
-        <v>262258.31</v>
+        <v>269310.07</v>
       </c>
       <c r="R139" s="188">
         <v>0</v>
@@ -32301,7 +32304,7 @@
         <v>529</v>
       </c>
       <c r="N141" s="187">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="O141" s="187">
         <v>0</v>
@@ -32310,7 +32313,7 @@
         <v>0</v>
       </c>
       <c r="Q141" s="188">
-        <v>43159.26</v>
+        <v>48295.199999999997</v>
       </c>
       <c r="R141" s="188">
         <v>0</v>
@@ -32388,7 +32391,7 @@
         <v>551</v>
       </c>
       <c r="N144" s="187">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="O144" s="187">
         <v>0</v>
@@ -32397,7 +32400,7 @@
         <v>0</v>
       </c>
       <c r="Q144" s="188">
-        <v>106820.55</v>
+        <v>113126.55</v>
       </c>
       <c r="R144" s="188">
         <v>0</v>
@@ -32475,7 +32478,7 @@
         <v>687</v>
       </c>
       <c r="N147" s="187">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="O147" s="187">
         <v>0</v>
@@ -32484,7 +32487,7 @@
         <v>0</v>
       </c>
       <c r="Q147" s="188">
-        <v>37782.85</v>
+        <v>55269.97</v>
       </c>
       <c r="R147" s="188">
         <v>0</v>
@@ -32533,7 +32536,7 @@
         <v>129</v>
       </c>
       <c r="N149" s="187">
-        <v>8676</v>
+        <v>8955</v>
       </c>
       <c r="O149" s="187">
         <v>0</v>
@@ -32542,7 +32545,7 @@
         <v>1</v>
       </c>
       <c r="Q149" s="188">
-        <v>1024804.87</v>
+        <v>1342765.15</v>
       </c>
       <c r="R149" s="188">
         <v>0</v>
@@ -32562,7 +32565,7 @@
         <v>632</v>
       </c>
       <c r="N150" s="187">
-        <v>699</v>
+        <v>708</v>
       </c>
       <c r="O150" s="187">
         <v>0</v>
@@ -32571,7 +32574,7 @@
         <v>0</v>
       </c>
       <c r="Q150" s="188">
-        <v>56884.44</v>
+        <v>63758.22</v>
       </c>
       <c r="R150" s="188">
         <v>0</v>
@@ -32649,7 +32652,7 @@
         <v>606</v>
       </c>
       <c r="N153" s="187">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="O153" s="187">
         <v>0</v>
@@ -32658,7 +32661,7 @@
         <v>0</v>
       </c>
       <c r="Q153" s="188">
-        <v>25605.61</v>
+        <v>26405.61</v>
       </c>
       <c r="R153" s="188">
         <v>0</v>
@@ -32736,7 +32739,7 @@
         <v>624</v>
       </c>
       <c r="N156" s="187">
-        <v>3475</v>
+        <v>3506</v>
       </c>
       <c r="O156" s="187">
         <v>0</v>
@@ -32745,7 +32748,7 @@
         <v>0</v>
       </c>
       <c r="Q156" s="188">
-        <v>193606.13</v>
+        <v>227800.59</v>
       </c>
       <c r="R156" s="188">
         <v>0</v>
@@ -32852,7 +32855,7 @@
         <v>639</v>
       </c>
       <c r="N160" s="187">
-        <v>289532</v>
+        <v>291474</v>
       </c>
       <c r="O160" s="187">
         <v>0</v>
@@ -32861,7 +32864,7 @@
         <v>3</v>
       </c>
       <c r="Q160" s="188">
-        <v>14117257.060000001</v>
+        <v>16760075.960000001</v>
       </c>
       <c r="R160" s="188">
         <v>0</v>
@@ -32881,7 +32884,7 @@
         <v>25</v>
       </c>
       <c r="N161" s="187">
-        <v>6261</v>
+        <v>6359</v>
       </c>
       <c r="O161" s="187">
         <v>0</v>
@@ -32890,7 +32893,7 @@
         <v>0</v>
       </c>
       <c r="Q161" s="188">
-        <v>2161517.7599999998</v>
+        <v>2306450.42</v>
       </c>
       <c r="R161" s="188">
         <v>0</v>
@@ -32910,7 +32913,7 @@
         <v>647</v>
       </c>
       <c r="N162" s="187">
-        <v>75758</v>
+        <v>76396</v>
       </c>
       <c r="O162" s="187">
         <v>0</v>
@@ -32919,7 +32922,7 @@
         <v>1</v>
       </c>
       <c r="Q162" s="188">
-        <v>9187784.75</v>
+        <v>10445015.98</v>
       </c>
       <c r="R162" s="188">
         <v>0</v>
@@ -32968,7 +32971,7 @@
         <v>654</v>
       </c>
       <c r="N164" s="187">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="O164" s="187">
         <v>0</v>
@@ -32977,7 +32980,7 @@
         <v>0</v>
       </c>
       <c r="Q164" s="188">
-        <v>14158.4</v>
+        <v>20575.400000000001</v>
       </c>
       <c r="R164" s="188">
         <v>0</v>
@@ -32997,7 +33000,7 @@
         <v>662</v>
       </c>
       <c r="N165" s="187">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O165" s="187">
         <v>0</v>
@@ -33006,7 +33009,7 @@
         <v>0</v>
       </c>
       <c r="Q165" s="188">
-        <v>151</v>
+        <v>609.5</v>
       </c>
       <c r="R165" s="188">
         <v>0</v>
@@ -33026,7 +33029,7 @@
         <v>671</v>
       </c>
       <c r="N166" s="187">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O166" s="187">
         <v>0</v>
@@ -33035,7 +33038,7 @@
         <v>0</v>
       </c>
       <c r="Q166" s="188">
-        <v>23295.95</v>
+        <v>23825.95</v>
       </c>
       <c r="R166" s="188">
         <v>0</v>
@@ -33113,7 +33116,7 @@
         <v>692</v>
       </c>
       <c r="N169" s="187">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O169" s="187">
         <v>0</v>
@@ -33122,7 +33125,7 @@
         <v>0</v>
       </c>
       <c r="Q169" s="188">
-        <v>1694.24</v>
+        <v>16294.24</v>
       </c>
       <c r="R169" s="188">
         <v>0</v>
@@ -37543,7 +37546,6 @@
       <c r="S570" s="188"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NC3D8uQLkEXga6kM1ET3E31Bhsejpveq41n9LD+gieFj9IItlc23FIDrqpkZSdhel1TOqQ+l1ye9BebkllNKOw==" saltValue="VHohcghjPyMYCN4bcraewg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="6">
     <mergeCell ref="N7:S7"/>
     <mergeCell ref="N8:P8"/>

</xml_diff>